<commit_message>
amended gerund verbs into BigBen
</commit_message>
<xml_diff>
--- a/English/BigBen/gerund verbs.xlsx
+++ b/English/BigBen/gerund verbs.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="199">
   <si>
     <t>to + V</t>
   </si>
@@ -311,9 +311,6 @@
   </si>
   <si>
     <t>make</t>
-  </si>
-  <si>
-    <t>изготовлять, творить</t>
   </si>
   <si>
     <t>mind</t>
@@ -610,9 +607,6 @@
     <t>will</t>
   </si>
   <si>
-    <t>делать, изготавливать</t>
-  </si>
-  <si>
     <t>auxiliary verb</t>
   </si>
   <si>
@@ -626,6 +620,15 @@
   </si>
   <si>
     <t>let + person</t>
+  </si>
+  <si>
+    <t>заставлять, делать</t>
+  </si>
+  <si>
+    <t>изготовлять, творить, делать</t>
+  </si>
+  <si>
+    <t>стартовать, начинать что-то делать</t>
   </si>
 </sst>
 </file>
@@ -1134,8 +1137,8 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,7 +1171,7 @@
       </c>
       <c r="H1" s="17"/>
       <c r="J1" s="16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K1" s="17"/>
     </row>
@@ -1193,10 +1196,10 @@
         <v>8</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1220,7 +1223,7 @@
         <v>14</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K3" s="19"/>
     </row>
@@ -1245,7 +1248,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K4" s="19"/>
     </row>
@@ -1264,16 +1267,16 @@
         <v>24</v>
       </c>
       <c r="F5" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>183</v>
-      </c>
       <c r="H5" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K5" s="20"/>
     </row>
@@ -1294,10 +1297,10 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="J6" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1317,10 +1320,10 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="J7" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1340,10 +1343,10 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="J8" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1361,10 +1364,10 @@
         <v>40</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1571,239 +1574,239 @@
         <v>93</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>94</v>
+        <v>197</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>142</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>149</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1811,10 +1814,10 @@
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
       <c r="D39" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1837,107 +1840,107 @@
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>161</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B44" s="10" t="s">
         <v>163</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>164</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E44" s="10" t="s">
         <v>165</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B45" s="11" t="s">
         <v>167</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>168</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E45" s="10" t="s">
         <v>169</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B46" s="11" t="s">
         <v>171</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>172</v>
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" s="10" t="s">
         <v>174</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>175</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B48" s="10" t="s">
         <v>177</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>178</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added clauses of contrast into BigBen
</commit_message>
<xml_diff>
--- a/English/BigBen/gerund verbs.xlsx
+++ b/English/BigBen/gerund verbs.xlsx
@@ -635,7 +635,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -665,15 +665,22 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="12.1"/>
+      <color rgb="FF282E3E"/>
       <name val="Arial"/>
       <charset val="204"/>
     </font>
     <font>
-      <sz val="12.1"/>
-      <color rgb="FF282E3E"/>
+      <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -775,7 +782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -783,33 +790,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -833,6 +817,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1137,8 +1147,8 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,800 +1167,800 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="16" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="16" t="s">
+      <c r="E1" s="19"/>
+      <c r="G1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="J1" s="16" t="s">
+      <c r="H1" s="8"/>
+      <c r="J1" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="K1" s="17"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="9" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="K3" s="19"/>
+      <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="K4" s="19"/>
+      <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="16"/>
+      <c r="D5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="K5" s="20"/>
+      <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="J6" s="4" t="s">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="J6" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="J7" s="4" t="s">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="J7" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="3" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="J8" s="4" t="s">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="J8" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="3" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="3" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="16"/>
+      <c r="D12" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="15" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="4" t="s">
+      <c r="C13" s="16"/>
+      <c r="D13" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="15" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="21"/>
+      <c r="D14" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="16"/>
+      <c r="D15" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="4" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="15" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="16"/>
+      <c r="D18" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="15" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="16"/>
+      <c r="D19" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="15" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="16"/>
+      <c r="D20" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="15" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="4" t="s">
+      <c r="C21" s="16"/>
+      <c r="D21" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="15" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="16"/>
+      <c r="D22" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="15" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="4" t="s">
+      <c r="C23" s="16"/>
+      <c r="D23" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="15" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="4" t="s">
+      <c r="C24" s="16"/>
+      <c r="D24" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="15" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="4" t="s">
+      <c r="C25" s="16"/>
+      <c r="D25" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="15" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="4" t="s">
+      <c r="C26" s="16"/>
+      <c r="D26" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="15" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="4" t="s">
+      <c r="C27" s="16"/>
+      <c r="D27" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="15" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="4" t="s">
+      <c r="C28" s="16"/>
+      <c r="D28" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="15" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="4" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="15" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="4" t="s">
+      <c r="C30" s="16"/>
+      <c r="D30" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="15" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="4" t="s">
+      <c r="C31" s="16"/>
+      <c r="D31" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="15" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="4" t="s">
+      <c r="C32" s="16"/>
+      <c r="D32" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="15" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="4" t="s">
+      <c r="C33" s="16"/>
+      <c r="D33" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="15" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="4" t="s">
+      <c r="C34" s="16"/>
+      <c r="D34" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="15" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="4" t="s">
+      <c r="C35" s="16"/>
+      <c r="D35" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="15" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="4" t="s">
+      <c r="C36" s="16"/>
+      <c r="D36" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="15" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="4" t="s">
+      <c r="C37" s="16"/>
+      <c r="D37" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="15" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="4" t="s">
+      <c r="C38" s="12"/>
+      <c r="D38" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="15" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="4" t="s">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="15" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9" t="s">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9" t="s">
+      <c r="C41" s="14"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="4" t="s">
+      <c r="C42" s="16"/>
+      <c r="D42" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="15" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="4" t="s">
+      <c r="C43" s="16"/>
+      <c r="D43" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="15" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="10" t="s">
+      <c r="C44" s="12"/>
+      <c r="D44" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="17" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="10" t="s">
+      <c r="C45" s="16"/>
+      <c r="D45" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="17" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="10" t="s">
+      <c r="C46" s="16"/>
+      <c r="D46" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="E46" s="15" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="10" t="s">
+      <c r="C47" s="12"/>
+      <c r="D47" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E47" s="17" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="10" t="s">
+      <c r="C48" s="12"/>
+      <c r="D48" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="17" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
+      <c r="A49" s="4"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
+      <c r="A50" s="5"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
+      <c r="A51" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1961,7 +1971,7 @@
     <mergeCell ref="K2:K5"/>
   </mergeCells>
   <pageMargins left="0.69652777777777797" right="0.70069444444444495" top="0.75138888888888899" bottom="0.75138888888888899" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
changed gerund verbs in BigBen
</commit_message>
<xml_diff>
--- a/English/BigBen/gerund verbs.xlsx
+++ b/English/BigBen/gerund verbs.xlsx
@@ -623,17 +623,19 @@
     <t>стартовать, начинать что-то делать</t>
   </si>
   <si>
-    <t>попытаться сделать что-то, прилагая усилие без гарантии достижения цели</t>
-  </si>
-  <si>
-    <t>попробовать сделать что-то разное
-для достижения цели</t>
-  </si>
-  <si>
     <t>propose</t>
   </si>
   <si>
     <t>предлагать (план решения и т.п.)</t>
+  </si>
+  <si>
+    <t>пытаться (сделать что-то, прилагая усилие без гарантии достижения цели)
+стараться</t>
+  </si>
+  <si>
+    <t>пытаться (сделать что-то разное
+для достижения цели)
+пробовать</t>
   </si>
 </sst>
 </file>
@@ -1152,8 +1154,8 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1653,10 +1655,10 @@
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1847,20 +1849,14 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8" t="s">
-        <v>0</v>
-      </c>
       <c r="C41" s="9"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>156</v>
+      <c r="A42" s="8"/>
+      <c r="B42" s="8" t="s">
+        <v>0</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="8"/>
@@ -1870,10 +1866,10 @@
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="10" t="s">
@@ -1885,10 +1881,10 @@
     </row>
     <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>163</v>
+        <v>159</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>160</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="10" t="s">
@@ -1898,12 +1894,12 @@
         <v>161</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>167</v>
+        <v>162</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>163</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="12" t="s">
@@ -1913,12 +1909,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
-        <v>170</v>
+    <row r="46" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>166</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>197</v>
+        <v>167</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="12" t="s">
@@ -1928,27 +1924,27 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>172</v>
+    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>199</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="12" t="s">
         <v>170</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
-        <v>174</v>
+      <c r="A48" s="10" t="s">
+        <v>171</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="12" t="s">
@@ -1959,7 +1955,12 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
+      <c r="A49" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>175</v>
+      </c>
       <c r="D49" s="12" t="s">
         <v>174</v>
       </c>

</xml_diff>